<commit_message>
Modify code + variable description
</commit_message>
<xml_diff>
--- a/data/input/variables_description.xlsx
+++ b/data/input/variables_description.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kacpergruca/Documents/Projekty/ING_Lions_Den_2024/data/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57E5CA1-78A0-7D4C-9ED0-5A5B5F9B5820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC93662-6DEC-384F-A768-67E38B4C0D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" xr2:uid="{F9B88B08-201A-4C85-9D6F-378EAD8AA833}"/>
   </bookViews>
@@ -1509,7 +1509,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>